<commit_message>
Measure 2019 ANSES deficit with 2019 Investment Account data; lower measured social security expenditure (lower pensions and lower transfers for disability pensions and security personnel social security schemes)
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Social_security_data/ANSES measured economic result detailed graph.xlsx
+++ b/Excel_files_for_MISSAR/Social_security_data/ANSES measured economic result detailed graph.xlsx
@@ -425,7 +425,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart81.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -437,9 +437,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.072342255186499"/>
-          <c:y val="0.0331011587032939"/>
-          <c:w val="0.884660862087499"/>
-          <c:h val="0.931324046348132"/>
+          <c:y val="0.0330686108579612"/>
+          <c:w val="0.884607115984091"/>
+          <c:h val="0.931258950657466"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -667,7 +667,7 @@
                   <c:v>0.0507048464919942</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0476951122067828</c:v>
+                  <c:v>0.045482634112618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1119,7 +1119,7 @@
                   <c:v>0.0270429026247307</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0261796371184609</c:v>
+                  <c:v>0.0262146924201451</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1346,7 +1346,7 @@
                   <c:v>-0.0763504580465942</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.0807087778924794</c:v>
+                  <c:v>-0.0745546912607249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1573,7 +1573,7 @@
                   <c:v>-0.0148720651077345</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.0115307335651721</c:v>
+                  <c:v>-0.0147840604707147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1798,7 +1798,7 @@
                   <c:v>-0.0111326724688934</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.0108797761936782</c:v>
+                  <c:v>-0.00804193239084517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1806,8 +1806,8 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="36805923"/>
-        <c:axId val="86832893"/>
+        <c:axId val="30574042"/>
+        <c:axId val="53448837"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -2036,7 +2036,7 @@
                   <c:v>-0.0182717978002125</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.0261904790563603</c:v>
+                  <c:v>-0.0226292983197961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,11 +2051,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="36805923"/>
-        <c:axId val="86832893"/>
+        <c:axId val="30574042"/>
+        <c:axId val="53448837"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36805923"/>
+        <c:axId val="30574042"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,14 +2083,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86832893"/>
+        <c:crossAx val="53448837"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86832893"/>
+        <c:axId val="53448837"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -2128,7 +2128,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36805923"/>
+        <c:crossAx val="30574042"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -2201,9 +2201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>95040</xdr:colOff>
+      <xdr:colOff>94680</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2212,7 +2212,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12229560" y="4211280"/>
-        <a:ext cx="6698160" cy="5530320"/>
+        <a:ext cx="6697800" cy="5529960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2232,11 +2232,11 @@
   </sheetPr>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N40" activeCellId="0" sqref="N40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R18" activeCellId="0" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.48"/>
@@ -3477,7 +3477,8 @@
         <v>2019</v>
       </c>
       <c r="H28" s="7" t="n">
-        <v>0.0476951122067828</v>
+        <f aca="false">B29</f>
+        <v>0.045482634112618</v>
       </c>
       <c r="I28" s="7" t="n">
         <f aca="false">D29</f>
@@ -3485,23 +3486,23 @@
       </c>
       <c r="J28" s="7" t="n">
         <f aca="false">SUM(C29:E29)-D29</f>
-        <v>0.0261796371184609</v>
+        <v>0.0262146924201451</v>
       </c>
       <c r="K28" s="8" t="n">
         <f aca="false">(B61+D61+G61)*-1</f>
-        <v>-0.0807087778924794</v>
+        <v>-0.0745546912607249</v>
       </c>
       <c r="L28" s="8" t="n">
         <f aca="false">(C61)*-1</f>
-        <v>-0.0115307335651721</v>
+        <v>-0.0147840604707147</v>
       </c>
       <c r="M28" s="8" t="n">
         <f aca="false">(F61+E61)*-1</f>
-        <v>-0.0108797761936782</v>
+        <v>-0.00804193239084517</v>
       </c>
       <c r="N28" s="8" t="n">
         <f aca="false">SUM(H28:M28)</f>
-        <v>-0.0261904790563603</v>
+        <v>-0.0226292983197961</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3509,50 +3510,50 @@
         <v>2019</v>
       </c>
       <c r="B29" s="7" t="n">
-        <v>0.0476951122067828</v>
+        <v>0.045482634112618</v>
       </c>
       <c r="C29" s="7" t="n">
-        <v>0.0259825128631984</v>
+        <v>0.025992153910621</v>
       </c>
       <c r="D29" s="7" t="n">
         <v>0.00305405926972561</v>
       </c>
       <c r="E29" s="7" t="n">
-        <v>0.000197124255262532</v>
+        <v>0.000222538509524099</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="10" t="n">
         <f aca="false">SUM(B29:E29)</f>
-        <v>0.0769288085949693</v>
+        <v>0.0747513858024887</v>
       </c>
       <c r="H31" s="10" t="n">
         <f aca="false">H28-H24</f>
-        <v>-0.00873460362313366</v>
+        <v>-0.0109470817172984</v>
       </c>
       <c r="I31" s="10" t="n">
         <f aca="false">I28-I24</f>
-        <v>-0.0130010488327954</v>
+        <v>-0.0130010488327955</v>
       </c>
       <c r="J31" s="10" t="n">
         <f aca="false">J28-J24</f>
-        <v>0.000788948270741375</v>
+        <v>0.000824003572425642</v>
       </c>
       <c r="K31" s="10" t="n">
         <f aca="false">K28-K24</f>
-        <v>-0.00359716804597789</v>
+        <v>0.0025569185857766</v>
       </c>
       <c r="L31" s="10" t="n">
         <f aca="false">L28-L24</f>
-        <v>0.000102116810493614</v>
+        <v>-0.00315121009504905</v>
       </c>
       <c r="M31" s="10" t="n">
         <f aca="false">M28-M24</f>
-        <v>0.00575860942608492</v>
+        <v>0.00859645322891793</v>
       </c>
       <c r="N31" s="10" t="n">
         <f aca="false">N28-N24</f>
-        <v>-0.0186831459945871</v>
+        <v>-0.0151219652580229</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,7 +3561,7 @@
       <c r="J32" s="0"/>
       <c r="L32" s="10" t="n">
         <f aca="false">SUM(K31:M31)</f>
-        <v>0.00226355819060065</v>
+        <v>0.00800216171964548</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,7 +3586,7 @@
       </c>
       <c r="J33" s="10" t="n">
         <f aca="false">H31+I31+J31+L32</f>
-        <v>-0.0186831459945871</v>
+        <v>-0.0151219652580228</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3598,7 +3599,7 @@
       <c r="G34" s="11"/>
       <c r="I34" s="10" t="n">
         <f aca="false">I31+H31</f>
-        <v>-0.0217356524559291</v>
+        <v>-0.0239481305500939</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3625,7 +3626,7 @@
       </c>
       <c r="I35" s="10" t="n">
         <f aca="false">J31+L32</f>
-        <v>0.00305250646134202</v>
+        <v>0.00882616529207112</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4309,26 +4310,26 @@
         <v>2019</v>
       </c>
       <c r="B61" s="8" t="n">
-        <v>0.0754137208560062</v>
+        <v>0.0705199284475343</v>
       </c>
       <c r="C61" s="8" t="n">
-        <v>0.0115307335651721</v>
+        <v>0.0147840604707147</v>
       </c>
       <c r="D61" s="8" t="n">
-        <v>0.0030177279977843</v>
+        <v>0.00271152710171896</v>
       </c>
       <c r="E61" s="8" t="n">
-        <v>0.00122106891178971</v>
+        <v>0.00125780693193743</v>
       </c>
       <c r="F61" s="8" t="n">
-        <v>0.00965870728188844</v>
+        <v>0.00678412545890775</v>
       </c>
       <c r="G61" s="8" t="n">
-        <v>0.00227732903868883</v>
+        <v>0.00132323571147159</v>
       </c>
       <c r="H61" s="10" t="n">
         <f aca="false">SUM(B29:E29)-SUM(B61:G61)</f>
-        <v>-0.0261904790563603</v>
+        <v>-0.0226292983197961</v>
       </c>
       <c r="I61" s="10"/>
     </row>

</xml_diff>

<commit_message>
Update CPI up to Oct. 2020, RIPTE Sep. 2020; coded historical IFE values, start considering hypothetical permanent IFE
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Social_security_data/ANSES measured economic result detailed graph.xlsx
+++ b/Excel_files_for_MISSAR/Social_security_data/ANSES measured economic result detailed graph.xlsx
@@ -425,7 +425,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -436,10 +436,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.072342255186499"/>
-          <c:y val="0.0330686108579612"/>
-          <c:w val="0.884607115984091"/>
-          <c:h val="0.931258950657466"/>
+          <c:x val="0.0723461435098092"/>
+          <c:y val="0.03307076362216"/>
+          <c:w val="0.884547164740661"/>
+          <c:h val="0.931189375691687"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1806,8 +1806,8 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="30574042"/>
-        <c:axId val="53448837"/>
+        <c:axId val="30786709"/>
+        <c:axId val="71749753"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -2051,11 +2051,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="30574042"/>
-        <c:axId val="53448837"/>
+        <c:axId val="30786709"/>
+        <c:axId val="71749753"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30574042"/>
+        <c:axId val="30786709"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,14 +2083,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53448837"/>
+        <c:crossAx val="71749753"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53448837"/>
+        <c:axId val="71749753"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -2128,7 +2128,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30574042"/>
+        <c:crossAx val="30786709"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -2201,9 +2201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>94680</xdr:colOff>
+      <xdr:colOff>94320</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2212,7 +2212,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12229560" y="4211280"/>
-        <a:ext cx="6697800" cy="5529960"/>
+        <a:ext cx="6697440" cy="5529600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2236,7 +2236,7 @@
       <selection pane="topLeft" activeCell="R18" activeCellId="0" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.48"/>

</xml_diff>

<commit_message>
Ran permanent IFE variants up to 2040, CPI and pension mobility; studied cost; corrected error on ANSES_measured_economic_result that reduced figurative expenses paid on 2019, deficit correctly reaches -2.58% GDP
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Social_security_data/ANSES measured economic result detailed graph.xlsx
+++ b/Excel_files_for_MISSAR/Social_security_data/ANSES measured economic result detailed graph.xlsx
@@ -425,7 +425,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart169.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -436,10 +436,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0723461435098092"/>
-          <c:y val="0.03307076362216"/>
-          <c:w val="0.884547164740661"/>
-          <c:h val="0.931189375691687"/>
+          <c:x val="0.0723500322511288"/>
+          <c:y val="0.0330729166666667"/>
+          <c:w val="0.884487207052247"/>
+          <c:h val="0.931119791666667"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1798,7 +1798,7 @@
                   <c:v>-0.0111326724688934</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.00804193239084517</c:v>
+                  <c:v>-0.0112040506102077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1806,8 +1806,8 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="30786709"/>
-        <c:axId val="71749753"/>
+        <c:axId val="51415867"/>
+        <c:axId val="48850129"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -2036,7 +2036,7 @@
                   <c:v>-0.0182717978002125</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.0226292983197961</c:v>
+                  <c:v>-0.0257914165391586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,11 +2051,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="30786709"/>
-        <c:axId val="71749753"/>
+        <c:axId val="51415867"/>
+        <c:axId val="48850129"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30786709"/>
+        <c:axId val="51415867"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,14 +2083,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71749753"/>
+        <c:crossAx val="48850129"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71749753"/>
+        <c:axId val="48850129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -2128,7 +2128,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30786709"/>
+        <c:crossAx val="51415867"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -2195,15 +2195,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>712080</xdr:colOff>
+      <xdr:colOff>712440</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>106560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>94320</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2211,8 +2211,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12229560" y="4211280"/>
-        <a:ext cx="6697440" cy="5529600"/>
+        <a:off x="12688200" y="4211640"/>
+        <a:ext cx="6697080" cy="5529240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2232,15 +2232,17 @@
   </sheetPr>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R18" activeCellId="0" sqref="R18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="12" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,11 +3500,11 @@
       </c>
       <c r="M28" s="8" t="n">
         <f aca="false">(F61+E61)*-1</f>
-        <v>-0.00804193239084517</v>
+        <v>-0.0112040506102077</v>
       </c>
       <c r="N28" s="8" t="n">
         <f aca="false">SUM(H28:M28)</f>
-        <v>-0.0226292983197961</v>
+        <v>-0.0257914165391586</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3549,11 +3551,11 @@
       </c>
       <c r="M31" s="10" t="n">
         <f aca="false">M28-M24</f>
-        <v>0.00859645322891793</v>
+        <v>0.00543433500955536</v>
       </c>
       <c r="N31" s="10" t="n">
         <f aca="false">N28-N24</f>
-        <v>-0.0151219652580229</v>
+        <v>-0.0182840834773854</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3561,7 +3563,7 @@
       <c r="J32" s="0"/>
       <c r="L32" s="10" t="n">
         <f aca="false">SUM(K31:M31)</f>
-        <v>0.00800216171964548</v>
+        <v>0.00484004350028291</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,10 +3588,10 @@
       </c>
       <c r="J33" s="10" t="n">
         <f aca="false">H31+I31+J31+L32</f>
-        <v>-0.0151219652580228</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-0.0182840834773853</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="35.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -3626,7 +3628,7 @@
       </c>
       <c r="I35" s="10" t="n">
         <f aca="false">J31+L32</f>
-        <v>0.00882616529207112</v>
+        <v>0.00566404707270855</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,14 +4324,14 @@
         <v>0.00125780693193743</v>
       </c>
       <c r="F61" s="8" t="n">
-        <v>0.00678412545890775</v>
+        <v>0.00994624367827031</v>
       </c>
       <c r="G61" s="8" t="n">
         <v>0.00132323571147159</v>
       </c>
       <c r="H61" s="10" t="n">
         <f aca="false">SUM(B29:E29)-SUM(B61:G61)</f>
-        <v>-0.0226292983197961</v>
+        <v>-0.0257914165391586</v>
       </c>
       <c r="I61" s="10"/>
     </row>

</xml_diff>